<commit_message>
FWMS - LoginPage Changes
</commit_message>
<xml_diff>
--- a/FWMS/docs/Open_Questions.xlsx
+++ b/FWMS/docs/Open_Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Sl No</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Where is administrator email configured?</t>
+  </si>
+  <si>
+    <t>How is OTP Generated and validated.</t>
+  </si>
+  <si>
+    <t>How is new Password Generated</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +526,9 @@
       <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -529,7 +537,9 @@
       <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>

</xml_diff>

<commit_message>
FWMS-Page Template and other artifacts.
</commit_message>
<xml_diff>
--- a/FWMS/docs/Open_Questions.xlsx
+++ b/FWMS/docs/Open_Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Sl No</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>How is new Password Generated</t>
+  </si>
+  <si>
+    <t>Main Menu not complete.</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +551,9 @@
       <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>

</xml_diff>

<commit_message>
FWMS - System Model changes.
</commit_message>
<xml_diff>
--- a/FWMS/docs/Open_Questions.xlsx
+++ b/FWMS/docs/Open_Questions.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="STOCK_SCREEN_MAPPING" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="112">
   <si>
     <t>Sl No</t>
   </si>
@@ -64,16 +63,311 @@
   </si>
   <si>
     <t>Main Menu not complete.</t>
+  </si>
+  <si>
+    <t>WMS_PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>WMS_PRODUCT_ID</t>
+  </si>
+  <si>
+    <t>WMS_PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>WMS_TICKER</t>
+  </si>
+  <si>
+    <t>WMS_RETUER_CODE</t>
+  </si>
+  <si>
+    <t>WMS_BLOOMBERG_CODE</t>
+  </si>
+  <si>
+    <t>WMS_ISIN_CODE</t>
+  </si>
+  <si>
+    <t>WMS_OTHER_CODE</t>
+  </si>
+  <si>
+    <t>WMS_OTHER_DESC</t>
+  </si>
+  <si>
+    <t>WMS_PRICE_UPDATE</t>
+  </si>
+  <si>
+    <t>WMS_COUNTRY</t>
+  </si>
+  <si>
+    <t>WMS_CURRENCY</t>
+  </si>
+  <si>
+    <t>WMS_STOCK_EXCHANGE</t>
+  </si>
+  <si>
+    <t>WMS_SECTOR</t>
+  </si>
+  <si>
+    <t>WMS_ASSET</t>
+  </si>
+  <si>
+    <t>WMS_BOND_ISSUE_NO</t>
+  </si>
+  <si>
+    <t>WMS_BOND_ISSUE_DATE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_MATURITY_DT</t>
+  </si>
+  <si>
+    <t>WMS_BOND_UNIT_PRICE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_RATE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_FREQUENCY</t>
+  </si>
+  <si>
+    <t>WMS_BOND_DIVISOR_DAYS_MONTH</t>
+  </si>
+  <si>
+    <t>WMS_BOND_DIVISOR_DAYS_YEAR</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_1ST_INTDATE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_2ND_INTDATE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_3RD_INTDATE</t>
+  </si>
+  <si>
+    <t>WMS_BOND_COUPON_4TH_INTDATE</t>
+  </si>
+  <si>
+    <t>WMS_PUT_CALL_FLAG</t>
+  </si>
+  <si>
+    <t>WMS_PUT_CALL_EXPIRY_DATE</t>
+  </si>
+  <si>
+    <t>WMS_PUT_CALL_LOTSIZE</t>
+  </si>
+  <si>
+    <t>WMS_PUT_CALL_SPRICE</t>
+  </si>
+  <si>
+    <t>WMS_PUT_CALL_STATUS</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_FUNDS_ISSUE</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_INHOUSE_3RD_FLAG</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_FUNDS_CLOSDED_OPEN</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_FUNDS_NAV_FLAG</t>
+  </si>
+  <si>
+    <t>WMS_COMMENTS</t>
+  </si>
+  <si>
+    <t>WMS_STATUS</t>
+  </si>
+  <si>
+    <t>WMS_ENTER_UID</t>
+  </si>
+  <si>
+    <t>WMS_ENTER_FPC</t>
+  </si>
+  <si>
+    <t>WMS_ENTER_DATE</t>
+  </si>
+  <si>
+    <t>WMS_LAST_UPDATE_UID</t>
+  </si>
+  <si>
+    <t>WMS_LAST_FPC</t>
+  </si>
+  <si>
+    <t>WMS_LAST_UPDATE_DATE</t>
+  </si>
+  <si>
+    <t>WMS_APPROVE_UID</t>
+  </si>
+  <si>
+    <t>WMS_APPROVE_FPC</t>
+  </si>
+  <si>
+    <t>WMS_APPROVE_DATE</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_FUNDS_VALUE</t>
+  </si>
+  <si>
+    <t>WMS_MUTUAL_IB_TYPE</t>
+  </si>
+  <si>
+    <t>WMS_SEDOL</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>UI FIELD</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>Serial Number. Might be a sequence generated</t>
+  </si>
+  <si>
+    <t>Stock Name</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Reuters Code</t>
+  </si>
+  <si>
+    <t>Bloomberg code</t>
+  </si>
+  <si>
+    <t>ISIN Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Stock Exchange</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Sedol</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Enter By</t>
+  </si>
+  <si>
+    <t>Last Updated By</t>
+  </si>
+  <si>
+    <t>Approved By</t>
+  </si>
+  <si>
+    <t>Approved Date</t>
+  </si>
+  <si>
+    <t>Last Updated Date</t>
+  </si>
+  <si>
+    <t>Entered Date</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>LOT Size</t>
+  </si>
+  <si>
+    <t>UI Attributes for which mapping is not found</t>
+  </si>
+  <si>
+    <t>Cusip</t>
+  </si>
+  <si>
+    <t>WMS_SNO</t>
+  </si>
+  <si>
+    <t>WMS_BOND</t>
+  </si>
+  <si>
+    <t>WMS_DATE</t>
+  </si>
+  <si>
+    <t>WMS_COUPEN</t>
+  </si>
+  <si>
+    <t>Issue No</t>
+  </si>
+  <si>
+    <t>Issue Date</t>
+  </si>
+  <si>
+    <t>Maturity Date</t>
+  </si>
+  <si>
+    <t>Unit Proce</t>
+  </si>
+  <si>
+    <t>Coupen Rate</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Bond Details</t>
+  </si>
+  <si>
+    <t>Payment Date 1st</t>
+  </si>
+  <si>
+    <t>Payment Date 2nd</t>
+  </si>
+  <si>
+    <t>Payment Date 3rd</t>
+  </si>
+  <si>
+    <t>Payment Date 4th</t>
+  </si>
+  <si>
+    <t>Divisor Days</t>
+  </si>
+  <si>
+    <t>Effect Date</t>
+  </si>
+  <si>
+    <t>Sequence?</t>
+  </si>
+  <si>
+    <t>Correct as per Sreeni</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,10 +414,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +734,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,9 +859,13 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -689,24 +998,675 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:I56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="G3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>34</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>35</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>38</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>39</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>40</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>41</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>42</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>43</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>44</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>45</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>46</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>47</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>48</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>49</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>50</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B54:C54"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FWMS - System UI changes.
</commit_message>
<xml_diff>
--- a/FWMS/docs/Open_Questions.xlsx
+++ b/FWMS/docs/Open_Questions.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="STOCK_SCREEN_MAPPING" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>Sl No</t>
   </si>
@@ -347,7 +347,28 @@
     <t>Sequence?</t>
   </si>
   <si>
-    <t>Correct as per Sreeni</t>
+    <t>SREENI - Ignore this field and no need to show this field</t>
+  </si>
+  <si>
+    <t>use WMS_OTHER_CODE</t>
+  </si>
+  <si>
+    <t>use WMS_BOND_DIVISOR_DAYS_YEAR</t>
+  </si>
+  <si>
+    <t>use for CUSIP</t>
+  </si>
+  <si>
+    <t>user for Divisor Days</t>
+  </si>
+  <si>
+    <t>I will send you code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this screen is master details - u should link to WMS_PRODUCT_ID field </t>
+  </si>
+  <si>
+    <t>Data Sent</t>
   </si>
   <si>
     <t>Closed</t>
@@ -734,7 +755,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,11 +881,11 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1002,14 +1023,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
@@ -1048,14 +1069,18 @@
       <c r="D2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>92</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -1072,7 +1097,9 @@
         <v>93</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
@@ -1156,7 +1183,9 @@
         <v>23</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -1166,7 +1195,9 @@
         <v>24</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
@@ -1176,7 +1207,9 @@
         <v>25</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
@@ -1330,7 +1363,9 @@
         <v>37</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
@@ -1340,7 +1375,9 @@
         <v>38</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
@@ -1397,7 +1434,9 @@
       <c r="C29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
@@ -1431,7 +1470,9 @@
         <v>46</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
@@ -1451,7 +1492,9 @@
         <v>48</v>
       </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
@@ -1461,7 +1504,9 @@
         <v>49</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
@@ -1471,7 +1516,9 @@
         <v>50</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
@@ -1481,7 +1528,9 @@
         <v>51</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
@@ -1527,7 +1576,9 @@
         <v>55</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
@@ -1561,7 +1612,9 @@
         <v>58</v>
       </c>
       <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
@@ -1594,7 +1647,9 @@
       <c r="C47" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
@@ -1616,7 +1671,9 @@
         <v>63</v>
       </c>
       <c r="D49" s="3"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
@@ -1626,7 +1683,9 @@
         <v>64</v>
       </c>
       <c r="D50" s="3"/>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
@@ -1653,6 +1712,9 @@
       <c r="C55" s="6" t="s">
         <v>91</v>
       </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56">
@@ -1660,6 +1722,9 @@
       </c>
       <c r="C56" s="6" t="s">
         <v>107</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FWMS - System UI and page template changes.
</commit_message>
<xml_diff>
--- a/FWMS/docs/Open_Questions.xlsx
+++ b/FWMS/docs/Open_Questions.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Stock Screen" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <t>Sl No</t>
   </si>
@@ -354,9 +354,6 @@
   </si>
   <si>
     <t>use WMS_BOND_DIVISOR_DAYS_YEAR</t>
-  </si>
-  <si>
-    <t>use for CUSIP</t>
   </si>
   <si>
     <t>user for Divisor Days</t>
@@ -753,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
@@ -881,11 +878,11 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1021,9 +1018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1067,7 @@
         <v>109</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>92</v>
@@ -1098,7 +1095,7 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1182,10 +1179,10 @@
       <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="D9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -1376,7 +1373,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1478,7 +1475,7 @@
       <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="3"/>

</xml_diff>